<commit_message>
Updating Gantt + Marathon PPT
</commit_message>
<xml_diff>
--- a/Documents/Project Gantt.xlsx
+++ b/Documents/Project Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitp\Documents\GitHub\MolOptimizer_Students_AY2023\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitp\Documents\GitHub\MolOpt_Students_2023\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5844E26-8329-4FEC-B26B-B94A43A5C64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F40FD9-14C4-4B3E-945F-49FBABB324EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A4C9E44-95D7-45D3-89CF-FCF08FF3DAE5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A4C9E44-95D7-45D3-89CF-FCF08FF3DAE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -158,12 +158,6 @@
     <t>system to the app</t>
   </si>
   <si>
-    <t>Adding multiple runs / running in</t>
-  </si>
-  <si>
-    <t>background functionality</t>
-  </si>
-  <si>
     <t>Creating database</t>
   </si>
   <si>
@@ -260,6 +254,21 @@
     <t xml:space="preserve"> servers</t>
   </si>
   <si>
+    <t>Finalize User/Runs</t>
+  </si>
+  <si>
+    <t>Managements</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Front &amp; Backend)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding multiple runs / </t>
+  </si>
+  <si>
+    <t>running queue functionality</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u/>
@@ -279,17 +288,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 10/3/23</t>
+      <t xml:space="preserve"> 22/4/23</t>
     </r>
-  </si>
-  <si>
-    <t>Finalize User/Runs</t>
-  </si>
-  <si>
-    <t>Managements</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (Front &amp; Backend)</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -600,81 +600,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,24 +616,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -732,18 +639,87 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -751,6 +727,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1070,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EA2AC0-1CA3-4028-B946-963609B74C8B}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,356 +1068,356 @@
     </row>
     <row r="3" spans="1:35" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11" t="s">
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11" t="s">
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="55"/>
+      <c r="P6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="12" t="s">
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12" t="s">
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11" t="s">
+      <c r="Y6" s="56"/>
+      <c r="Z6" s="55"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="12" t="s">
+      <c r="AC6" s="55"/>
+      <c r="AD6" s="55"/>
+      <c r="AE6" s="55"/>
+      <c r="AF6" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="12"/>
+      <c r="AG6" s="56"/>
+      <c r="AH6" s="56"/>
+      <c r="AI6" s="56"/>
     </row>
     <row r="7" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16" t="s">
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="16" t="s">
+      <c r="I7" s="34"/>
+      <c r="J7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="17" t="s">
+      <c r="K7" s="35"/>
+      <c r="L7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="18"/>
-      <c r="N7" s="16" t="s">
+      <c r="M7" s="35"/>
+      <c r="N7" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="18"/>
-      <c r="P7" s="13" t="s">
+      <c r="O7" s="35"/>
+      <c r="P7" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="16" t="s">
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="18"/>
-      <c r="V7" s="16" t="s">
+      <c r="U7" s="35"/>
+      <c r="V7" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="18"/>
-      <c r="X7" s="16" t="s">
+      <c r="W7" s="35"/>
+      <c r="X7" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="22" t="s">
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="43"/>
-      <c r="AE7" s="44"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="29"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="24" t="s">
+      <c r="I8" s="54"/>
+      <c r="J8" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="25" t="s">
+      <c r="K8" s="41"/>
+      <c r="L8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="28"/>
-      <c r="N8" s="24" t="s">
+      <c r="M8" s="41"/>
+      <c r="N8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="28"/>
-      <c r="T8" s="24" t="s">
+      <c r="O8" s="41"/>
+      <c r="T8" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="U8" s="28"/>
-      <c r="V8" s="24" t="s">
+      <c r="U8" s="41"/>
+      <c r="V8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="W8" s="28"/>
-      <c r="X8" s="24" t="s">
+      <c r="W8" s="41"/>
+      <c r="X8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="Y8" s="28"/>
-      <c r="AB8" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="47"/>
+      <c r="Y8" s="41"/>
+      <c r="AB8" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="32"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="24" t="s">
+      <c r="I9" s="37"/>
+      <c r="J9" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="20" t="s">
+      <c r="K9" s="41"/>
+      <c r="L9" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="38"/>
+      <c r="N9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="19" t="s">
+      <c r="O9" s="38"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="W9" s="21"/>
-      <c r="X9" s="19" t="s">
+      <c r="W9" s="38"/>
+      <c r="X9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="21"/>
+      <c r="Y9" s="38"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="21"/>
+      <c r="K10" s="38"/>
+      <c r="AA10" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB10" s="49"/>
+      <c r="AD10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE10" s="12"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="V11" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="W11" s="35"/>
+      <c r="AA11" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB11" s="51"/>
+      <c r="AD11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE11" s="14"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="H12" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="35"/>
+      <c r="V12" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="W12" s="41"/>
+      <c r="AA12" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB12" s="53"/>
+      <c r="AD12" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE12" s="16"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="H13" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="38"/>
+      <c r="V13" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="W13" s="38"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="H15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="35"/>
+      <c r="N15" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="O15" s="47"/>
+      <c r="T15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="39"/>
+      <c r="Z15" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA15" s="25"/>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="25"/>
+      <c r="AD15" s="25"/>
+      <c r="AE15" s="25"/>
+      <c r="AF15" s="25"/>
+      <c r="AG15" s="39"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="T11" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="U11" s="58"/>
-      <c r="V11" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="W11" s="37"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A12" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="H12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="18"/>
-      <c r="T12" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="U12" s="59"/>
-      <c r="V12" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="W12" s="39"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="55"/>
-      <c r="H13" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="21"/>
-      <c r="T13" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="U13" s="61"/>
-      <c r="V13" s="40" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="L16" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="38"/>
+      <c r="N16" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="43"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="N17" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="W13" s="41"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="H15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" s="18"/>
-      <c r="N15" s="26" t="s">
+      <c r="O17" s="45"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="AB18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="10"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AD19" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="O15" s="27"/>
-      <c r="T15" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="U15" s="34"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA15" s="34"/>
-      <c r="AB15" s="34"/>
-      <c r="AC15" s="34"/>
-      <c r="AD15" s="34"/>
-      <c r="AE15" s="34"/>
-      <c r="AF15" s="34"/>
-      <c r="AG15" s="35"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="L16" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="21"/>
-      <c r="N16" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="O16" s="30"/>
-      <c r="X16" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y16" s="39"/>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A17" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="N17" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" s="32"/>
-      <c r="X17" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y17" s="41"/>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="X19" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="AE19" s="9"/>
       <c r="AF19" s="9"/>
@@ -1441,33 +1426,46 @@
       <c r="AI19" s="10"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="O20" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="50"/>
+      <c r="O20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="19"/>
     </row>
     <row r="22" spans="1:35" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="AD19:AI19"/>
-    <mergeCell ref="Z15:AG15"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="AB6:AE6"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA11:AB11"/>
     <mergeCell ref="AB7:AE7"/>
     <mergeCell ref="AB8:AE8"/>
     <mergeCell ref="L12:O12"/>
@@ -1483,43 +1481,30 @@
     <mergeCell ref="T8:U8"/>
     <mergeCell ref="T9:U9"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="X16:Y16"/>
-    <mergeCell ref="X15:Y15"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="T15:W15"/>
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="N15:O15"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="T12:U12"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="X19:AC19"/>
-    <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="AD19:AI19"/>
+    <mergeCell ref="Z15:AG15"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="AD11:AE11"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="AB18:AG18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated statistics & Docs
</commit_message>
<xml_diff>
--- a/Documents/Project Gantt.xlsx
+++ b/Documents/Project Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitp\Documents\GitHub\MolOpt_Students_2023\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F40FD9-14C4-4B3E-945F-49FBABB324EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600AEB0-DAB9-4342-AE6F-F6E321A1B381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A4C9E44-95D7-45D3-89CF-FCF08FF3DAE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A4C9E44-95D7-45D3-89CF-FCF08FF3DAE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 22/4/23</t>
+      <t xml:space="preserve"> 30/4/23</t>
     </r>
   </si>
 </sst>
@@ -582,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -591,31 +591,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -639,60 +672,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,31 +693,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1055,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EA2AC0-1CA3-4028-B946-963609B74C8B}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC23" sqref="AC23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,357 +1063,357 @@
     </row>
     <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55" t="s">
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="56" t="s">
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56" t="s">
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Y6" s="56"/>
-      <c r="Z6" s="55"/>
-      <c r="AA6" s="55"/>
-      <c r="AB6" s="55" t="s">
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="55"/>
-      <c r="AD6" s="55"/>
-      <c r="AE6" s="55"/>
-      <c r="AF6" s="56" t="s">
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="56"/>
-      <c r="AH6" s="56"/>
-      <c r="AI6" s="56"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
     </row>
     <row r="7" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="33" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="33" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="34" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="35"/>
-      <c r="N7" s="33" t="s">
+      <c r="M7" s="15"/>
+      <c r="N7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="35"/>
-      <c r="P7" s="24" t="s">
+      <c r="O7" s="15"/>
+      <c r="P7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="33" t="s">
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="35"/>
-      <c r="V7" s="33" t="s">
+      <c r="U7" s="15"/>
+      <c r="V7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="35"/>
-      <c r="X7" s="33" t="s">
+      <c r="W7" s="15"/>
+      <c r="X7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="24" t="s">
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="27" t="s">
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AC7" s="28"/>
-      <c r="AD7" s="28"/>
-      <c r="AE7" s="29"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="24"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="40" t="s">
+      <c r="I8" s="20"/>
+      <c r="J8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="54" t="s">
+      <c r="K8" s="21"/>
+      <c r="L8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="41"/>
-      <c r="N8" s="40" t="s">
+      <c r="M8" s="21"/>
+      <c r="N8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="41"/>
-      <c r="T8" s="40" t="s">
+      <c r="O8" s="21"/>
+      <c r="T8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="U8" s="41"/>
-      <c r="V8" s="40" t="s">
+      <c r="U8" s="21"/>
+      <c r="V8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="W8" s="41"/>
-      <c r="X8" s="40" t="s">
+      <c r="W8" s="21"/>
+      <c r="X8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="Y8" s="41"/>
-      <c r="AB8" s="30" t="s">
+      <c r="Y8" s="21"/>
+      <c r="AB8" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" s="31"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="32"/>
+      <c r="AC8" s="26"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="27"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="40" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="41"/>
-      <c r="L9" s="37" t="s">
+      <c r="K9" s="21"/>
+      <c r="L9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="38"/>
-      <c r="N9" s="36" t="s">
+      <c r="M9" s="18"/>
+      <c r="N9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="38"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="36" t="s">
+      <c r="O9" s="18"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="W9" s="38"/>
-      <c r="X9" s="36" t="s">
+      <c r="W9" s="18"/>
+      <c r="X9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="38"/>
+      <c r="Y9" s="18"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="AA10" s="48" t="s">
+      <c r="K10" s="18"/>
+      <c r="AA10" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AB10" s="49"/>
-      <c r="AD10" s="11" t="s">
+      <c r="AB10" s="15"/>
+      <c r="AD10" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="AE10" s="12"/>
+      <c r="AE10" s="48"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="V11" s="33" t="s">
+      <c r="B11" s="31"/>
+      <c r="V11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="W11" s="35"/>
-      <c r="AA11" s="50" t="s">
+      <c r="W11" s="15"/>
+      <c r="AA11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="AB11" s="51"/>
-      <c r="AD11" s="13" t="s">
+      <c r="AB11" s="21"/>
+      <c r="AD11" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="AE11" s="14"/>
+      <c r="AE11" s="46"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="H12" s="33" t="s">
+      <c r="B12" s="34"/>
+      <c r="H12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="33" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="35"/>
-      <c r="V12" s="40" t="s">
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="15"/>
+      <c r="V12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="W12" s="41"/>
-      <c r="AA12" s="52" t="s">
+      <c r="W12" s="21"/>
+      <c r="AA12" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AB12" s="53"/>
-      <c r="AD12" s="15" t="s">
+      <c r="AB12" s="18"/>
+      <c r="AD12" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="AE12" s="16"/>
+      <c r="AE12" s="50"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="H13" s="36" t="s">
+      <c r="B13" s="35"/>
+      <c r="H13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="36" t="s">
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="38"/>
-      <c r="V13" s="36" t="s">
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="18"/>
+      <c r="V13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="W13" s="38"/>
+      <c r="W13" s="18"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="33" t="s">
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="M15" s="35"/>
-      <c r="N15" s="46" t="s">
+      <c r="M15" s="15"/>
+      <c r="N15" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="47"/>
-      <c r="T15" s="24" t="s">
+      <c r="O15" s="41"/>
+      <c r="T15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="39"/>
-      <c r="Z15" s="24" t="s">
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="12"/>
+      <c r="Z15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
-      <c r="AD15" s="25"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="39"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="12"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="L16" s="36" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="L16" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="38"/>
-      <c r="N16" s="42" t="s">
+      <c r="M16" s="18"/>
+      <c r="N16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="43"/>
+      <c r="O16" s="37"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="N17" s="44" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="N17" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="45"/>
+      <c r="O17" s="39"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="AB18" s="8" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="AB18" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="10"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="12"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="AD19" s="8" t="s">
+      <c r="AD19" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="9"/>
-      <c r="AI19" s="10"/>
+      <c r="AE19" s="43"/>
+      <c r="AF19" s="43"/>
+      <c r="AG19" s="43"/>
+      <c r="AH19" s="43"/>
+      <c r="AI19" s="44"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="19"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="30"/>
     </row>
     <row r="22" spans="1:35" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -1440,6 +1422,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="AB18:AG18"/>
+    <mergeCell ref="AD19:AI19"/>
+    <mergeCell ref="Z15:AG15"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="AD11:AE11"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="AB7:AE7"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="AF6:AI6"/>
     <mergeCell ref="D7:G7"/>
@@ -1456,55 +1487,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AB7:AE7"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="X7:Y7"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="AD19:AI19"/>
-    <mergeCell ref="Z15:AG15"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="AD11:AE11"/>
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="T15:W15"/>
-    <mergeCell ref="AB18:AG18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalize All Project Documents
</commit_message>
<xml_diff>
--- a/Documents/Project Gantt.xlsx
+++ b/Documents/Project Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitp\Documents\GitHub\MolOpt_Students_2023\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7600AEB0-DAB9-4342-AE6F-F6E321A1B381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F85809-6660-44AB-97E6-57926B1E58D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A4C9E44-95D7-45D3-89CF-FCF08FF3DAE5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A4C9E44-95D7-45D3-89CF-FCF08FF3DAE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 30/4/23</t>
+      <t xml:space="preserve"> 3/6/23</t>
     </r>
   </si>
 </sst>
@@ -582,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -591,10 +591,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,49 +612,37 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,31 +687,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1063,357 +1045,357 @@
     </row>
     <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:35" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8" t="s">
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9" t="s">
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9" t="s">
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8" t="s">
+      <c r="Y6" s="44"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="9" t="s">
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="43"/>
+      <c r="AF6" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
+      <c r="AG6" s="44"/>
+      <c r="AH6" s="44"/>
+      <c r="AI6" s="44"/>
     </row>
     <row r="7" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="40"/>
+      <c r="J7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="14" t="s">
+      <c r="K7" s="19"/>
+      <c r="L7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="15"/>
-      <c r="N7" s="13" t="s">
+      <c r="M7" s="19"/>
+      <c r="N7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="10" t="s">
+      <c r="O7" s="19"/>
+      <c r="P7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="13" t="s">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="U7" s="15"/>
-      <c r="V7" s="13" t="s">
+      <c r="U7" s="19"/>
+      <c r="V7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="15"/>
-      <c r="X7" s="13" t="s">
+      <c r="W7" s="19"/>
+      <c r="X7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="10" t="s">
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="22" t="s">
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="24"/>
+      <c r="AC7" s="40"/>
+      <c r="AD7" s="40"/>
+      <c r="AE7" s="19"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="19" t="s">
+      <c r="I8" s="42"/>
+      <c r="J8" s="20" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="21"/>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="42" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="21"/>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="O8" s="21"/>
-      <c r="T8" s="19" t="s">
+      <c r="T8" s="20" t="s">
         <v>29</v>
       </c>
       <c r="U8" s="21"/>
-      <c r="V8" s="19" t="s">
+      <c r="V8" s="20" t="s">
         <v>14</v>
       </c>
       <c r="W8" s="21"/>
-      <c r="X8" s="19" t="s">
+      <c r="X8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="Y8" s="21"/>
-      <c r="AB8" s="25" t="s">
+      <c r="AB8" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="27"/>
+      <c r="AC8" s="41"/>
+      <c r="AD8" s="41"/>
+      <c r="AE8" s="23"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="19" t="s">
+      <c r="I9" s="41"/>
+      <c r="J9" s="20" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="21"/>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="16" t="s">
+      <c r="M9" s="23"/>
+      <c r="N9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="16" t="s">
+      <c r="O9" s="23"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="W9" s="18"/>
-      <c r="X9" s="16" t="s">
+      <c r="W9" s="23"/>
+      <c r="X9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="18"/>
+      <c r="Y9" s="23"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="18"/>
-      <c r="AA10" s="13" t="s">
+      <c r="K10" s="23"/>
+      <c r="AA10" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AB10" s="15"/>
-      <c r="AD10" s="47" t="s">
+      <c r="AB10" s="19"/>
+      <c r="AD10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AE10" s="48"/>
+      <c r="AE10" s="9"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="V11" s="13" t="s">
+      <c r="B11" s="29"/>
+      <c r="V11" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="W11" s="15"/>
-      <c r="AA11" s="19" t="s">
+      <c r="W11" s="19"/>
+      <c r="AA11" s="20" t="s">
         <v>59</v>
       </c>
       <c r="AB11" s="21"/>
-      <c r="AD11" s="45" t="s">
+      <c r="AD11" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AE11" s="46"/>
+      <c r="AE11" s="25"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="H12" s="13" t="s">
+      <c r="B12" s="32"/>
+      <c r="H12" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="13" t="s">
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="15"/>
-      <c r="V12" s="19" t="s">
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="19"/>
+      <c r="V12" s="20" t="s">
         <v>41</v>
       </c>
       <c r="W12" s="21"/>
-      <c r="AA12" s="16" t="s">
+      <c r="AA12" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AB12" s="18"/>
-      <c r="AD12" s="49" t="s">
+      <c r="AB12" s="23"/>
+      <c r="AD12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AE12" s="50"/>
+      <c r="AE12" s="11"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="H13" s="16" t="s">
+      <c r="B13" s="33"/>
+      <c r="H13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="16" t="s">
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="18"/>
-      <c r="V13" s="16" t="s">
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="23"/>
+      <c r="V13" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="W13" s="18"/>
+      <c r="W13" s="23"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="13" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="40" t="s">
+      <c r="M15" s="19"/>
+      <c r="N15" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="41"/>
-      <c r="T15" s="10" t="s">
+      <c r="O15" s="39"/>
+      <c r="T15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="12"/>
-      <c r="Z15" s="10" t="s">
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="14"/>
+      <c r="Z15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="12"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="13"/>
+      <c r="AG15" s="14"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="L16" s="16" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="L16" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="18"/>
-      <c r="N16" s="36" t="s">
+      <c r="M16" s="23"/>
+      <c r="N16" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="37"/>
+      <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="N17" s="38" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="N17" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="39"/>
+      <c r="O17" s="37"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="AB18" s="10" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="AB18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="12"/>
+      <c r="AC18" s="13"/>
+      <c r="AD18" s="13"/>
+      <c r="AE18" s="13"/>
+      <c r="AF18" s="13"/>
+      <c r="AG18" s="14"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="AD19" s="42" t="s">
+      <c r="AD19" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AE19" s="43"/>
-      <c r="AF19" s="43"/>
-      <c r="AG19" s="43"/>
-      <c r="AH19" s="43"/>
-      <c r="AI19" s="44"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="16"/>
+      <c r="AI19" s="17"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="O20" s="28" t="s">
+      <c r="O20" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="30"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="28"/>
     </row>
     <row r="22" spans="1:35" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -1422,29 +1404,32 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="AD10:AE10"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="T15:W15"/>
-    <mergeCell ref="AB18:AG18"/>
-    <mergeCell ref="AD19:AI19"/>
-    <mergeCell ref="Z15:AG15"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="AD11:AE11"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="AB6:AE6"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA11:AB11"/>
     <mergeCell ref="AB7:AE7"/>
     <mergeCell ref="AB8:AE8"/>
     <mergeCell ref="L12:O12"/>
@@ -1461,32 +1446,29 @@
     <mergeCell ref="T9:U9"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="AB18:AG18"/>
+    <mergeCell ref="AD19:AI19"/>
+    <mergeCell ref="Z15:AG15"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="AD11:AE11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>